<commit_message>
file download 기능 추가_pyhton을 활용한 flask 실습
</commit_message>
<xml_diff>
--- a/python_ex/day05/result_en.xlsx
+++ b/python_ex/day05/result_en.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3번째 Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2번째 Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Prudential Financial, personal information of 2.5 million people stolen... Alfab ransomware group</t>
+          <t>China-linked cyber espionage group Velvet Ant exploits Cisco NX-OS zero-day vulnerability to attack… Caution</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157434</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157415</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Prudential Financial, an American multinational financial services company, was hacked in February and the personal information of more than 2.5 million people was leaked. This figure far exceeds the initially reported number of 36,000. This data breach occurred on February 4, 2024. Prudential Financial detected this the next day and immediately took action. According to Form 8-K filed with the U.S. Securities and Exchange Commission (SEC), the attackers gained access to the company's administrative and user data, as well as the accounts of employees and contractors. Meanwhile, the BlackCat ransomware group took advantage of this attack.</t>
+          <t>Velvet Ant, a Chinese-linked cyber espionage group, is exploiting a zero-day vulnerability in Cisco NX-OS software, according to a recent report from cybersecurity firm Sygnia.CVE-2024-20399 The vulnerability being tracked is a command injection vulnerability that could allow an authenticated, local attacker to execute arbitrary commands with root privileges on the underlying operating system of an affected device. This vulnerability, with a CVSS score of 6.0, affects certain vulnerabilities in Cisco NX-OS software. Due to insufficient validation of arguments passed to the configuration CLI command.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -471,24 +471,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-07-03 17:15:40</t>
+          <t>2024-07-03 12:02:26</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>KISA-Korea Aerospace Research Institute signs business agreement to strengthen aerospace security</t>
+          <t>Kaspersky “Cyber ​​Threat Intelligence (TI) product line and training will be sold as before in the U.S.”</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157428</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157408</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Korea Internet &amp; Security Agency (President Lee Sang-jung, hereinafter referred to as KISA) signed a business agreement (MOU) to strengthen security with the Korea Aerospace Research Institute (President Lee Sang-ryul, hereinafter referred to as 'Aerospace Research Institute') at the Korea Aerospace Research Institute's Daejeon headquarters on Wednesday, July 3. KISA made efforts to spread security awareness by collaborating with private aerospace industry officials, such as holding an 'Aerospace and Aviation Convergence Security Seminar' in October last year to share the latest aerospace security trends and policy directions. This agreement Accordingly, both organizations will strengthen the security of aerospace companies and products, develop and verify aerospace security models, train aerospace security personnel and raise awareness, and</t>
+          <t>The U.S. Department of Commerce's Bureau of Industry and Security (BIS) last week announced measures to ban Kaspersky's U.S. subsidiary from directly or indirectly providing security software in the United States. However, sales and training of Threat Intelligence (TI) products are possible as before. Kaspersky will be prohibited from selling software, excluding TI products and training, to U.S. consumers and companies starting July 20. However, we will continue to provide software and anti-virus signature updates to existing customers until September 29. Additionally, we will provide current individual and business customers with an appropriate replacement software within 100 days to ensure there are no gaps in security protection.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -498,24 +498,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2024-07-03 16:47:35</t>
+          <t>2024-07-03 09:40:42</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ransomware payouts soar and the limitations of legacy MFA</t>
+          <t>Prudential Financial, personal information of 2.5 million people stolen... Alfab ransomware group</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157423</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157434</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cyber ​​security threats have been increasing rapidly recently. According to the Sophos "State of Ransomware 2024" report, average ransom payouts increased 500% last year, reaching an average of $2 million, up from $400,000 in 2023. Additionally, according to the RISK &amp; INSURANCE report, the median ransom demand in 2023 surged from $1.4 million in 2022 to $20 million, and the actual payment amount increased from $335,000 to $6.5 million. ◆Increasing ransomware payouts Factor 1. Targeting of CybercriminalsCybercriminals use maximum</t>
+          <t>Prudential Financial, an American multinational financial services company, was hacked in February and the personal information of more than 2.5 million people was leaked. This figure far exceeds the initially reported number of 36,000. This data breach occurred on February 4, 2024. Prudential Financial detected this the next day and immediately took action. According to Form 8-K filed with the U.S. Securities and Exchange Commission (SEC), the attackers gained access to the company's administrative and user data, as well as the accounts of employees and contractors. Meanwhile, the BlackCat ransomware group took advantage of this attack.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -525,24 +525,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2024-07-03 15:51:47</t>
+          <t>2024-07-03 17:15:40</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>China-linked cyber espionage group Velvet Ant exploits Cisco NX-OS zero-day vulnerability to attack… Caution</t>
+          <t>Google conducts kvmCTF to strengthen KVM hypervisor security... Pays $250,000 for zero-day vulnerabilities</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157415</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157414</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Velvet Ant, a Chinese-linked cyber espionage group, is exploiting a zero-day vulnerability in Cisco NX-OS software, according to a recent report from cybersecurity firm Sygnia.CVE-2024-20399 The vulnerability being tracked is a command injection vulnerability that could allow an authenticated, local attacker to execute arbitrary commands with root privileges on the underlying operating system of an affected device. This vulnerability, with a CVSS score of 6.0, affects certain vulnerabilities in Cisco NX-OS software. Due to insufficient validation of arguments passed to the configuration CLI command.</t>
+          <t>Google announced the introduction of a new Vulnerability Reward Program (VRP), kvmCTF, to enhance the security of its Kernel-based Virtual Machine (KVM) hypervisor. First announced in October 2023, the program identifies vulnerabilities within KVM and Aim to correct. KVM plays an important role in consumer and enterprise environments and is used on a variety of platforms, including Android and Google Cloud Platform. KVM is an open source hypervisor with over 17 years of development history that enables Linux to operate as a hypervisor. Google is the master of KVM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -552,24 +552,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2024-07-03 12:02:26</t>
+          <t>2024-07-03 11:21:41</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Google conducts kvmCTF to strengthen KVM hypervisor security... Pays $250,000 for zero-day vulnerabilities</t>
+          <t>Soaring ransomware payouts and the limitations of legacy MFA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157414</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157423</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Google announced the introduction of a new Vulnerability Reward Program (VRP), kvmCTF, to enhance the security of its Kernel-based Virtual Machine (KVM) hypervisor. First announced in October 2023, the program identifies vulnerabilities within KVM and Aim to correct. KVM plays an important role in consumer and enterprise environments and is used on a variety of platforms, including Android and Google Cloud Platform. KVM is an open source hypervisor with over 17 years of development history that enables Linux to operate as a hypervisor. Google is the master of KVM</t>
+          <t>Cyber ​​security threats have been increasing rapidly recently. According to the Sophos "State of Ransomware 2024" report, average ransom payouts increased 500% last year, reaching an average of $2 million, up from $400,000 in 2023. Additionally, according to the RISK &amp; INSURANCE report, the median ransom demand in 2023 surged from $1.4 million in 2022 to $20 million, and the actual payment amount increased from $335,000 to $6.5 million. ◆Increasing ransomware payouts Factor 1. Targeting of CybercriminalsCybercriminals use maximum</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -579,24 +579,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2024-07-03 11:21:41</t>
+          <t>2024-07-03 15:51:47</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>National Intelligence Service holds a meeting on ‘Public Cloud Security Policy’ with domestic and foreign industries</t>
+          <t>Iroun &amp; Company, a generative AI security company, selected as Deeptech Tips Fast Track</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157396</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157412</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>On July 2, the National Intelligence Service, together with the Digital Platform Government Committee, held a meeting at the National Cyber ​​Security Center (Pangyo) at the National Cyber ​​Security Center (Pangyo), inviting executives from major domestic and foreign cloud industries, Korea Information Security Industry Association, and other related associations to a meeting on the topic of “Multi-layer security system and cloud security policy.” At the meeting on this day, the National Intelligence Service explained the direction of promoting a multi-layered security system, which is an ongoing network security policy improvement plan in relation to the expansion of AI-cloud technology adoption in the public sector, and discussed cloud construction plans and security standards accordingly. In addition, the government's active support and support for the revitalization of the security industry along with questions and answers about security policies such as cloud</t>
+          <t>Lee Roun &amp; Company (CEO Yoon Du-sik), Korea's first generative AI security company, was finally selected for the fast track 'Deep Tech Tips' private investment-led technology startup support program of the Ministry of SMEs and Startups (hereinafter referred to as the Ministry of SMEs and Startups). Lee Roun &amp; Company received seed investment from Mark &amp; ​​Company and the Yoonmin Creative Investment Foundation in February 2024, and was selected as DeepTech TIPS after being recommended by TIPS operator Mark &amp; ​​Company. DeepTech TIPS is a promising start in the top 10 new industries. As part of the Super Gap Startup 1000+ project announced by the Ministry of SMEs and Startups to select and foster businesses, selected companies will receive KRW 1.5 billion in research and development (R&amp;D) expenses, as well as commercialization and overseas support.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -606,24 +606,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2024-07-02 17:46:02</t>
+          <t>2024-07-03 10:48:24</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>The 11th Software Development Security Contest held</t>
+          <t>JSI Lab launches X-ITM, Auto ML-based threat response solution</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157393</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157417</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The Korea Internet &amp; Security Agency (President Lee Sang-jung, hereinafter referred to as KISA) announced on July 2 (Tuesday) that it will hold the '11th Software Development Security Contest' together with the Ministry of Science and ICT (Minister Lee Jong-ho, hereinafter referred to as the Ministry of Science and ICT). Software Development Security It prevents accidents such as hacking by considering security from the software development stage, and its importance has recently been growing along with software supply chain security. The ‘Software Development Security Contest’ has been held every year since 2014 to raise awareness of the importance of software development security and to discover talent. This contest is designed to “create software development security.”</t>
+          <t>JSI LAB (CEO Taeyong Ha), a company specializing in security AI, announced that it has launched X-ITM 1.0, an Auto ML-based threat response solution. JSI LAB conducts Auto ML and AI work. In the security field, predicting security events based on transformers, recognizing hacking through deep learning-based image recognition, predicting security incidents through statistical-based predictions, predicting unknown or unrecognized patterns through unsupervised learning, and predicting patterns that are unknown or unrecognized through existing ESM or Load patterns into SIEM and improve the accuracy of security events through supervised learning using existing patterns and labeling.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -633,24 +633,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2024-07-02 17:21:09</t>
+          <t>2024-07-03 14:00:04</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>'Supply Chain Security Workshop' held on July 11th (Thursday) - 12th (Friday)</t>
+          <t>RaonSecure wins contract for ‘mobile ID construction and expansion service’ project</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157386</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157418</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>The Supply Chain Security Research Association (Chairman Professor Manhee Lee) announced that it will hold a supply chain security workshop from Thursday, July 11th to Friday, July 12th. Recently, cases of cyber hacking through vulnerable supply chains have increased rapidly, and supply chain security has been strengthened, especially in the United States. Movements to increase the level of national cybersecurity are progressing rapidly. However, in Korea, although awareness of the need for supply chain security has been formed to some extent, it has not yet garnered the attention of many people. Universities and research institutes are responsible for developing core technologies for supply chain security, and the industry is responsible for commercializing this technology. Lastly, to apply it across the country</t>
+          <t>Raon Secure (CEO Soon-Hyung Lee, Jeong-Ah Lee) announced that it has won an order for the ‘Mobile ID Construction and Expansion Service’ project ordered by the Korea Minting and Security Minting Corporation to build a blockchain-based mobile resident registration card issuance system by the Ministry of the Interior and Safety. Raon Secure is issuing this mobile resident registration card. We provide OmniOne Enterprise, a blockchain-based digital ID platform, for system development and are responsible for the mobile security sector required when issuing resident registration cards in a mobile environment. RaonSecure's blockchain-based digital technology has previously been applied to mobile driver's licenses and mobile national veterans registration cards. OmniOne Enterprise, an identity platform, is a FIDO (biometric</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -660,24 +660,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2024-07-02 16:19:51</t>
+          <t>2024-07-03 14:16:46</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Phishing email discovered that induces users to directly execute malicious code</t>
+          <t>AhnLab selected as a supplier for the ‘2024 ICT Small and Medium Business Information Protection Support Project’...Recruiting demand companies</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157381</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157420</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>AhnLab (CEO Seok-gyun Kang) recently discovered a phishing email that induces users to directly execute malicious code and urged users to be cautious. In the cases recently discovered by AhnLab, the attacker first responded with content such as handling costs and reviewing operating guidelines. An attached file (.html) was distributed along with a disguised phishing email. When the user opens the attached file to check its contents, a fake page elaborately disguised as an MS Word document and an information message appear. The information message states, “The online version of the document program is not installed,” and “To view the document, click the How to Fix button. It says “Click ” so that the user can</t>
+          <t>AhnLab (CEO Seok-gyun Kang) announced that it has been selected as a security solution supplier for the '2024 ICT Small and Medium Business Information Protection Support Project (hereinafter referred to as 'Support Project') and is recruiting companies in demand. This support project includes ◇ information security consulting and security solution support ◇ cloud It is divided into two areas, including support for basic security services (SECaaS). AhnLab provides SaaS (Software as a Service) type security management solution for small and medium-sized businesses across each field, including the 'AhnLab Office Security' product line (3 types); Network security solution ‘AhnLab TrusGuard’ 50B-70B model</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -687,24 +687,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2024-07-02 15:29:13</t>
+          <t>2024-07-03 14:40:29</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>The Ministry of Science and ICT operates Information Protection Month, including international conferences and exhibitions, throughout the month of July.</t>
+          <t>KISA-Korea Aerospace Research Institute signs business agreement to strengthen aerospace security</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157375</t>
+          <t>https://www.dailysecu.com/news/articleView.html?idxno=157428</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>The Ministry of Science and ICT (Minister Lee Jong-ho, hereinafter referred to as 'MSIT'), the Korea Information Security Industry Association (Chairman Cho Young-cheol, hereinafter referred to as 'KISIA'), and the Korea Internet &amp; Security Agency (President Lee Sang-joong, hereinafter referred to as 'KISA') are 'protecting by strengthening global cybersecurity.' Information Security Month is being held throughout July under the theme of 'Everyone's Trust!'. 'Information Protection Month' is held to raise public security awareness and spread a culture of information protection practice in response to increasing cyber threats. It is held every year in July, and various commemorative events have been held, including awards to those who have contributed to information protection and campaigns to raise public awareness. This year, the area of ​​information protection has been opened to the public.</t>
+          <t>Korea Internet &amp; Security Agency (President Lee Sang-jung, hereinafter referred to as KISA) signed a business agreement (MOU) to strengthen security with the Korea Aerospace Research Institute (President Lee Sang-ryul, hereinafter referred to as 'Aerospace Research Institute') at the Korea Aerospace Research Institute's Daejeon headquarters on Wednesday, July 3. KISA made efforts to spread security awareness by collaborating with private aerospace industry officials, such as holding an 'Aerospace and Aviation Convergence Security Seminar' in October last year to share the latest aerospace security trends and policy directions. This agreement Accordingly, both organizations will strengthen the security of aerospace companies and products, develop and verify aerospace security models, train aerospace security personnel and raise awareness, and</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -714,277 +714,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2024-07-02 14:23:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Recruiting key leaders... Hyundai AutoEver, speed of strengthening security and SW competitiveness</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157348</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Hyundai AutoEver is accelerating its efforts to strengthen its competitiveness in the cyber security and software (SW) business by recruiting two key executives who are attracting attention from major IT companies such as Naver and Socar. Hyundai AutoEver has hired Executive Director Choi Won-hyuk, formerly of Naver Cloud, and Socar announced on the 1st that it had recruited Managing Director Ji Doo-hyeon and appointed him as Chief Security Officer (CISO) and Head of SW Development Center, respectively. Legal Affairs Director Shim Min-jeong was promoted to managing director and became the first female executive at Hyundai Autoever. Managing Director Choi Won-hyuk, who was appointed Chief Security Officer (CISO), recorded numerous 'industry firsts' with innovative attempts in the field of information and data protection over 22 years. A security expert who has written</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2024-07-01 18:31:24</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>56% of downtime incidents are caused by security incidents such as phishing, and 44% are caused by software failures.</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157324</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Splunk, a leading company in the field of cybersecurity and observability, announced a global report, 'The Hidden Costs of Downtime', together with Oxford Economics, a British economic analysis agency. The report was suddenly downloaded. It deals with direct costs and costs that are not directly revealed due to time. According to the report, when large global companies included in the ‘Forbes Global 2000’ experience downtime due to unexpected digital environment failures, the downtime cost incurred is $400 billion per year, which is 9% of total revenue.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2024-07-01 11:21:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Security threats increase as many organizations fail to secure overall API visibility</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157319</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Cloudflare's 2024 App Security Report highlights that online threats are growing significantly and that many organizations are struggling with outdated security approaches. With APIs now accounting for more than half of Internet traffic, their security is becoming more important. Zero-day vulnerabilities and rapid exploitation One of the biggest highlights of the report is that new zero-day vulnerabilities are being exploited at a record pace. Cloudflare observed a case where this vulnerability was exploited 22 minutes after the proof of concept (PoC) was released. These rapid exploits allow organizations to be proactive and take action to stay ahead of attackers.</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2024-07-01 10:57:06</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Logpresso “Evolution of APT attacks using open source tools… Credential theft has been confirmed in many cases in Korea as well.”</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157314</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Logpresso (CEO Bong-yeol Yang), a cloud SIEM specialist company, announced on the 1st that it has published the 'June 2024 CTI (Cyber ​​Threat Intelligence) Monthly Report'. Logpresso prepared the June CTI report based on data collected last month. , we covered cases of APT attacks that are evolving using open source attack tools and various cybersecurity issues that occurred in May. In this report, we disclosed an in-depth analysis of the XenoRAT attack targeting Korea and the GoStealer attack targeting the Indian Air Force.</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2024-07-01 09:48:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>North Korean hacker group Kim Suki conducts hacking activities using new malicious Chrome extension</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157311</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>North Korean cyber hacking group Kimsuky has been found to be using a new malicious Google Chrome extension to steal sensitive information. This extension is primarily being used as part of intelligence-gathering activities targeting South Korean academics studying North Korean political issues. ◆TRANSLATEXT, a new cyber espionage toolZscaler ThreatLabz discovered this malicious program in early March. Activity was observed. This extension, named TRANSLATEXT, allows you to enter your email address, username, password,</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2024-06-30 15:39:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Google blocks Entrust certificates starting in November due to security issues... Companies using Entrust certificates are in crisis</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157310</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Google announced that it will block websites that use TLS server certificates issued by Entrust starting November 1, 2024. This action was cited as a result of Entrust's repeated failures to comply with regulations and a decline in trust due to security issues. Google's published incident reports over the past few years have revealed serious problems with Entrust's behavioral patterns, which have led to its ability to, It said that confidence in its reliability and integrity has decreased. This measure will apply to Chrome browser versions 127 and higher for Windows, macOS, ChromeOS, Android, and Linux.</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2024-06-30 15:20:02</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Next-generation security leader training program (BoB) 13th launch ceremony completed successfully</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157302</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>The Korea Institute of Information Technology (President Jun-sang Yoo, hereinafter referred to as KITRI) held an inauguration ceremony for the 13th class of the ‘Next Generation Security Leader Training Program (Best of the Best, hereinafter referred to as BoB)’ at the Grand Ballroom on the 12th floor of the CCMM Building in Yeongdeungpo-gu, Seoul on Friday, June 28 at 14:00. The launch ceremony was held. At the site of the launch ceremony were Second Vice Minister of Science and ICT Kang Do-hyun, People Power Party lawmaker Ahn Cheol-soo, Democratic Party lawmaker Park Hong-geun, People Power lawmaker Song Seok-jun, People Power lawmaker Cho Bae-sook, People Power lawmaker Lim Jong-deuk, People Power Party lawmaker Ko Dong-jin, Lim Jong-in, Special Adviser to the President on Cyber, Oh-jun Yoon, 3rd Deputy Director of the National Intelligence Service, Shin Yong-seok, Cyber ​​Security Secretary of the National Security Office, and Director Park Joon-hong.</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2024-06-28 16:42:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>The 13th Korea Internet Governance Forum (KrIGF) will be held in 2024.</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157301</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>The Korea Internet &amp; Security Agency (President Lee Sang-jung, hereinafter referred to as ‘KISA’) held the ‘13th Korea Internet Governance Forum (KrIGF)’ together with 17 Internet-related institutions, organizations, and companies, including the Multilateral Internet Governance Council (Chairman Lee Dong-man). ' will be jointly held at the Francis Education Center on June 28. The Korea Internet Governance Forum has been held every year since 2012 to promote discussion among various stakeholders on major public policy issues related to the Internet. The 13th forum was ‘Multi-stakeholder of safety and human rights in the era of artificial intelligence.</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2024-06-28 16:31:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Nuri Lab, 'Offsec Cyber ​​Attack Training Competition' 2024, held from July 9th to 10th</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157276</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>From July 9 to July 10, 2024, an opportunity to verify the skills of cybersecurity experts will be held. Global cyber security company Nuri Lab (CEO Won-hyuk Choi, Jeong-ho Park) held an 'OffSec Cyber ​​Attack Training Competition' to prepare for ever-evolving cyber attacks and hacking threats in celebration of the launch of OffSec in Korea and Information Protection Day. He said he would. This competition will be held from 9:00 AM on July 9, 2024 to 6:00 PM on July 10, 2024, and participants will develop defense skills, threat hunting skills, and breach response skills through training exercises from an attacker's perspective (offensive security).</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2024-06-28 13:52:59</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>TeamViewer suffers cyber attack by APT hacking group... Users beware</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>https://www.dailysecu.com/news/articleView.html?idxno=157260</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>TeamViewer, a famous remote access software company, announced on the 26th that its corporate environment was breached due to a cyber attack, and a cybersecurity company claimed that the attack was caused by an APT hacking group. TeamViewer said, "June 2024 “On Wednesday the 26th, our security team detected unusual activity in our internal corporate IT environment, immediately activated response teams and processes, began an investigation with world-renowned cybersecurity experts, and implemented necessary recovery measures.” .He continued, “TeamViewer’s internal corporate IT environment is completely separated from the product environment. The current product environment is</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Reporter Gil Min-kwon</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2024-06-28 06:25:44</t>
+          <t>2024-07-03 16:47:35</t>
         </is>
       </c>
     </row>

</xml_diff>